<commit_message>
Final Version of CityVille
Final version of CityVille with FaceBook integration
</commit_message>
<xml_diff>
--- a/CityVille Daily Update Log.xlsx
+++ b/CityVille Daily Update Log.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -236,6 +236,12 @@
   </si>
   <si>
     <t>postReport()</t>
+  </si>
+  <si>
+    <t>Integrate Facebook</t>
+  </si>
+  <si>
+    <t>Add Share Button</t>
   </si>
 </sst>
 </file>
@@ -841,6 +847,35 @@
         <v>68</v>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" s="5">
+        <v>42198.0</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="D71" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="D72" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>